<commit_message>
combined and cleaned up the 2020-2021 data files, including updating the taxonomy file
</commit_message>
<xml_diff>
--- a/Data/phytoplankton/2021/DFW_Phyto_Samples_2021_all.xlsx
+++ b/Data/phytoplankton/2021/DFW_Phyto_Samples_2021_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\AQUATICS\AQUATIC ARCHIVE\DATA ARCHIVES\CDWR - ALL PROJECTS\CDWR YOLO\PHYTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\SMSCG\Data\phytoplankton\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7CCB422-8339-46FB-8E62-D0869B5DAF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ECD0BC-11AA-42FC-9C52-86D521284F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21330" yWindow="3915" windowWidth="14310" windowHeight="11385" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17640" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Info" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5040" uniqueCount="322">
   <si>
     <t>Cyclotella sp.</t>
   </si>
@@ -980,9 +980,6 @@
     <t>BSA.YOLO-66</t>
   </si>
   <si>
-    <t>10/7/211</t>
-  </si>
-  <si>
     <t>BSA.YOLO-67</t>
   </si>
   <si>
@@ -1289,15 +1286,7 @@
     <cellStyle name="Normal_Sheet1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal_Tulsa - species list" xfId="4" xr:uid="{DC1583C4-8A8C-4FAB-8787-02496ED9652E}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1652,8 +1641,8 @@
   <dimension ref="A1:BO888"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B865" sqref="B865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15848,7 +15837,7 @@
         <v>102</v>
       </c>
       <c r="AC183" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD183" s="8" t="s">
         <v>100</v>
@@ -16000,7 +15989,7 @@
         <v>102</v>
       </c>
       <c r="AC186" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD186" s="8" t="s">
         <v>44</v>
@@ -16128,7 +16117,7 @@
         <v>102</v>
       </c>
       <c r="AC188" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD188" s="8" t="s">
         <v>149</v>
@@ -16255,7 +16244,7 @@
         <v>102</v>
       </c>
       <c r="AC190" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD190" s="8" t="s">
         <v>50</v>
@@ -16347,7 +16336,7 @@
         <v>102</v>
       </c>
       <c r="AC191" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD191" s="8" t="s">
         <v>44</v>
@@ -16476,7 +16465,7 @@
         <v>102</v>
       </c>
       <c r="AC193" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD193" s="8" t="s">
         <v>50</v>
@@ -16586,7 +16575,7 @@
         <v>102</v>
       </c>
       <c r="AC194" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD194" s="8" t="s">
         <v>50</v>
@@ -16776,7 +16765,7 @@
         <v>102</v>
       </c>
       <c r="AC195" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD195" s="8" t="s">
         <v>50</v>
@@ -16880,7 +16869,7 @@
         <v>102</v>
       </c>
       <c r="AC196" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD196" s="8" t="s">
         <v>44</v>
@@ -41602,7 +41591,7 @@
         <v>102</v>
       </c>
       <c r="AC539" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AD539" s="8" t="s">
         <v>44</v>
@@ -41724,7 +41713,7 @@
         <v>102</v>
       </c>
       <c r="AC541" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AD541" s="8" t="s">
         <v>175</v>
@@ -41906,7 +41895,7 @@
         <v>102</v>
       </c>
       <c r="AC545" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AD545" s="8" t="s">
         <v>101</v>
@@ -42041,7 +42030,7 @@
         <v>102</v>
       </c>
       <c r="AC547" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AD547" s="8" t="s">
         <v>50</v>
@@ -62497,7 +62486,7 @@
         <v>102</v>
       </c>
       <c r="AC839" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD839" s="8" t="s">
         <v>175</v>
@@ -62679,7 +62668,7 @@
         <v>102</v>
       </c>
       <c r="AC843" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD843" s="8" t="s">
         <v>50</v>
@@ -62842,7 +62831,7 @@
         <v>102</v>
       </c>
       <c r="AC846" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD846" s="8" t="s">
         <v>50</v>
@@ -62937,7 +62926,7 @@
         <v>102</v>
       </c>
       <c r="AC847" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD847" s="8" t="s">
         <v>117</v>
@@ -63060,7 +63049,7 @@
         <v>102</v>
       </c>
       <c r="AC849" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD849" s="8" t="s">
         <v>101</v>
@@ -63183,7 +63172,7 @@
         <v>102</v>
       </c>
       <c r="AC851" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD851" s="8" t="s">
         <v>117</v>
@@ -63306,7 +63295,7 @@
         <v>102</v>
       </c>
       <c r="AC853" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD853" s="8" t="s">
         <v>101</v>
@@ -63441,7 +63430,7 @@
         <v>102</v>
       </c>
       <c r="AC855" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD855" s="8" t="s">
         <v>50</v>
@@ -63631,7 +63620,7 @@
         <v>102</v>
       </c>
       <c r="AC856" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD856" s="8" t="s">
         <v>203</v>
@@ -63716,8 +63705,8 @@
       <c r="A859" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B859" s="36" t="s">
-        <v>316</v>
+      <c r="B859" s="36">
+        <v>44476</v>
       </c>
       <c r="C859" s="37">
         <v>0.46875</v>
@@ -63779,7 +63768,7 @@
         <v>5</v>
       </c>
       <c r="AA859" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AB859" s="7" t="s">
         <v>102</v>
@@ -63868,8 +63857,8 @@
       <c r="A862" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B862" s="36" t="s">
-        <v>316</v>
+      <c r="B862" s="36">
+        <v>44476</v>
       </c>
       <c r="C862" s="37">
         <v>0.46875</v>
@@ -63931,7 +63920,7 @@
         <v>5</v>
       </c>
       <c r="AA862" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AB862" s="7" t="s">
         <v>102</v>
@@ -63990,8 +63979,8 @@
       <c r="A864" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B864" s="36" t="s">
-        <v>316</v>
+      <c r="B864" s="36">
+        <v>44476</v>
       </c>
       <c r="C864" s="37">
         <v>0.46875</v>
@@ -64053,7 +64042,7 @@
         <v>5</v>
       </c>
       <c r="AA864" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AB864" s="7" t="s">
         <v>102</v>
@@ -64112,8 +64101,8 @@
       <c r="A866" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B866" s="36" t="s">
-        <v>316</v>
+      <c r="B866" s="36">
+        <v>44476</v>
       </c>
       <c r="C866" s="37">
         <v>0.46875</v>
@@ -64181,7 +64170,7 @@
         <v>56</v>
       </c>
       <c r="AA866" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AB866" s="7" t="s">
         <v>102</v>
@@ -64371,7 +64360,7 @@
         <v>5</v>
       </c>
       <c r="AA867" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB867" s="7" t="s">
         <v>102</v>
@@ -64493,7 +64482,7 @@
         <v>5</v>
       </c>
       <c r="AA869" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB869" s="7" t="s">
         <v>102</v>
@@ -64621,7 +64610,7 @@
         <v>5</v>
       </c>
       <c r="AA871" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB871" s="7" t="s">
         <v>102</v>
@@ -64725,7 +64714,7 @@
         <v>56</v>
       </c>
       <c r="AA872" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB872" s="7" t="s">
         <v>102</v>
@@ -64915,7 +64904,7 @@
         <v>5</v>
       </c>
       <c r="AA873" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB873" s="7" t="s">
         <v>91</v>
@@ -65049,7 +65038,7 @@
         <v>5</v>
       </c>
       <c r="AA875" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB875" s="7" t="s">
         <v>91</v>
@@ -65201,7 +65190,7 @@
         <v>5</v>
       </c>
       <c r="AA878" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB878" s="7" t="s">
         <v>91</v>
@@ -65380,7 +65369,7 @@
         <v>5</v>
       </c>
       <c r="AA881" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB881" s="7" t="s">
         <v>91</v>
@@ -65532,7 +65521,7 @@
         <v>5</v>
       </c>
       <c r="AA884" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB884" s="7" t="s">
         <v>91</v>
@@ -65660,7 +65649,7 @@
         <v>5</v>
       </c>
       <c r="AA886" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB886" s="7" t="s">
         <v>91</v>
@@ -65801,7 +65790,7 @@
         <v>56</v>
       </c>
       <c r="AA888" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB888" s="7" t="s">
         <v>91</v>
@@ -65926,7 +65915,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BO11">
-    <sortCondition sortBy="cellColor" ref="P2:P11" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="P2:P11" dxfId="0"/>
   </sortState>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>